<commit_message>
Cattermole CO estimation of liver blood flow added
</commit_message>
<xml_diff>
--- a/experimental_data/GEC/Lange2011.xlsx
+++ b/experimental_data/GEC/Lange2011.xlsx
@@ -44,7 +44,7 @@
     <t>age</t>
   </si>
   <si>
-    <t>GEC</t>
+    <t>GECkg</t>
   </si>
   <si>
     <t>lan2011</t>
@@ -270,7 +270,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -607,11 +607,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="14521211"/>
-        <c:axId val="46466157"/>
+        <c:axId val="91592444"/>
+        <c:axId val="94881076"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="14521211"/>
+        <c:axId val="91592444"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -645,11 +645,11 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="46466157"/>
+        <c:crossAx val="94881076"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="46466157"/>
+        <c:axId val="94881076"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -684,7 +684,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="14521211"/>
+        <c:crossAx val="91592444"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -723,14 +723,14 @@
 <xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>847080</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>477000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>648360</xdr:colOff>
+      <xdr:colOff>398880</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>3960</xdr:rowOff>
     </xdr:to>
@@ -763,13 +763,13 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>848880</xdr:colOff>
+      <xdr:colOff>599400</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>93240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>216000</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>779040</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>85680</xdr:rowOff>
     </xdr:to>
@@ -804,13 +804,13 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>361800</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>203400</xdr:rowOff>
+      <xdr:rowOff>212400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>1030680</xdr:colOff>
+      <xdr:colOff>1031040</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>131040</xdr:rowOff>
+      <xdr:rowOff>140040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -818,8 +818,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10077120" y="680040"/>
-        <a:ext cx="4732920" cy="3737880"/>
+        <a:off x="10326600" y="689040"/>
+        <a:ext cx="4733280" cy="3737880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -840,7 +840,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100">
-      <selection activeCell="G46" activeCellId="0" pane="topLeft" sqref="G46"/>
+      <selection activeCell="J45" activeCellId="0" pane="topLeft" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -848,7 +848,8 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.7142857142857"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3265306122449"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.7448979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.0561224489796"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.5969387755102"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.7040816326531"/>
     <col collapsed="false" hidden="false" max="15" min="8" style="0" width="11.5204081632653"/>
@@ -862,7 +863,6 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.35" outlineLevel="0" r="3">
       <c r="A3" s="2" t="s">

</xml_diff>